<commit_message>
New project V3.0 Se agrega una clase nueva para extraer datos de un excel. Ahora son colocadas las variables del excel por medio de getters y setters.
</commit_message>
<xml_diff>
--- a/data/Browser Data.xlsx
+++ b/data/Browser Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MiguelTorres\Documents\SELENIUM PROJECTS\Gradle-Tutorial-IntelliJIDEA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C8129F-7EA8-49E3-BEF6-A600286D60FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35481BF-7C9F-490D-B351-54E5C2E25E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1DF2AA4-C70B-484D-9A4D-659B17A6743A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1DF2AA4-C70B-484D-9A4D-659B17A6743A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="118">
   <si>
     <t>chrome</t>
   </si>
@@ -222,6 +222,174 @@
   </si>
   <si>
     <t>fghfhg</t>
+  </si>
+  <si>
+    <t>vvv</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>cdfg</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>gf</t>
+  </si>
+  <si>
+    <t>dgfh</t>
+  </si>
+  <si>
+    <t>gfhjg</t>
+  </si>
+  <si>
+    <t>hjg</t>
+  </si>
+  <si>
+    <t>ghj</t>
+  </si>
+  <si>
+    <t>jgh</t>
+  </si>
+  <si>
+    <t>sfg</t>
+  </si>
+  <si>
+    <t>hjkh</t>
+  </si>
+  <si>
+    <t>e56tert</t>
+  </si>
+  <si>
+    <t>gffg</t>
+  </si>
+  <si>
+    <t>hfghfg</t>
+  </si>
+  <si>
+    <t>hgj</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Test Case Name3</t>
+  </si>
+  <si>
+    <t>Test Case Name1</t>
+  </si>
+  <si>
+    <t>Test Case Name2</t>
+  </si>
+  <si>
+    <t>Test Case Name4</t>
+  </si>
+  <si>
+    <t>Test Case Name5</t>
+  </si>
+  <si>
+    <t>Test Case Name6</t>
+  </si>
+  <si>
+    <t>Test Case Name7</t>
+  </si>
+  <si>
+    <t>Test Case Name8</t>
+  </si>
+  <si>
+    <t>Test Case Name9</t>
+  </si>
+  <si>
+    <t>Test Case Name10</t>
+  </si>
+  <si>
+    <t>Test Case Name11</t>
+  </si>
+  <si>
+    <t>Test Case Name12</t>
+  </si>
+  <si>
+    <t>Test Case Name13</t>
+  </si>
+  <si>
+    <t>Test Case Name14</t>
+  </si>
+  <si>
+    <t>Test Case Name15</t>
+  </si>
+  <si>
+    <t>Test Case Name16</t>
+  </si>
+  <si>
+    <t>Test Case Name17</t>
+  </si>
+  <si>
+    <t>Test Case Name18</t>
+  </si>
+  <si>
+    <t>Test Case Name19</t>
+  </si>
+  <si>
+    <t>Test Case Name20</t>
+  </si>
+  <si>
+    <t>Test Case Name21</t>
+  </si>
+  <si>
+    <t>Test Case Name22</t>
+  </si>
+  <si>
+    <t>Test Case Name23</t>
+  </si>
+  <si>
+    <t>Test Case Name24</t>
+  </si>
+  <si>
+    <t>Test Case Name25</t>
+  </si>
+  <si>
+    <t>Test Case Name26</t>
+  </si>
+  <si>
+    <t>Test Case Name27</t>
+  </si>
+  <si>
+    <t>Test Case Name28</t>
+  </si>
+  <si>
+    <t>Test Case Name29</t>
+  </si>
+  <si>
+    <t>Test Case Name30</t>
+  </si>
+  <si>
+    <t>Test Case Name31</t>
+  </si>
+  <si>
+    <t>Test Case Name32</t>
+  </si>
+  <si>
+    <t>Test Case Name33</t>
+  </si>
+  <si>
+    <t>Test Case Name34</t>
+  </si>
+  <si>
+    <t>Test Case Name35</t>
+  </si>
+  <si>
+    <t>Test Case Name36</t>
+  </si>
+  <si>
+    <t>Test Case Name37</t>
   </si>
 </sst>
 </file>
@@ -579,298 +747,545 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED1848B-F90F-4D0C-9B98-DA8C8FF5F5A7}">
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2:AE4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>43</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>44</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>45</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>46</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>47</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>49</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>50</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>51</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>52</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>53</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>54</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>55</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>56</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>57</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>21</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>20</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>22</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>22</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="AA7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="AA13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="AA18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" t="s">
+        <v>60</v>
+      </c>
+      <c r="O20" t="s">
+        <v>60</v>
+      </c>
+      <c r="R20" t="s">
+        <v>60</v>
+      </c>
+      <c r="V20" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>110</v>
+      </c>
+      <c r="K31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="M32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>112</v>
+      </c>
+      <c r="O33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20" t="s">
-        <v>60</v>
-      </c>
-      <c r="N20" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>60</v>
-      </c>
-      <c r="U20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>